<commit_message>
Added SIMS year division script + quick fix for false year placements
</commit_message>
<xml_diff>
--- a/Oto_sizes_2022.xlsx
+++ b/Oto_sizes_2022.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timor\Nextcloud2\Timo\BODDENHECHT\Chapter 2\Stats\Otolith data prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF19DE1D-6482-4159-9C45-0A6E86D86E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10815C0-CBCA-4D50-8503-DD4D691E5E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9767340-0B6C-47AF-9169-7574FCBB593D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Otolith</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>#T</t>
+  </si>
+  <si>
+    <t>G-BH-91588</t>
+  </si>
+  <si>
+    <t>#G</t>
   </si>
 </sst>
 </file>
@@ -570,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6807CB-2649-438F-8066-E770D2D2DC49}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -991,6 +997,20 @@
         <v>1200</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3607</v>
+      </c>
+      <c r="D30">
+        <v>1200</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C64">
     <sortCondition ref="A2:A64"/>

</xml_diff>